<commit_message>
Final Changes in Front-End, updated Back-End
</commit_message>
<xml_diff>
--- a/Ressourcen/To-do Liste.xlsx
+++ b/Ressourcen/To-do Liste.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Desktop\Desktop\Wiss Sachen\3. Semester\Module 294\Aufgaben\8B-SideQuest\LB-Projekt-M294-295_Ethan-Shrestha\Projektdokumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Desktop\Desktop\Wiss Sachen\3. Semester\Module 294\Aufgaben\8B-SideQuest\LB-Projekt-M294-295_Ethan-Shrestha\Ressourcen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3388C8-6DA7-42D2-86EF-73729F7A3E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F44F5D-E08C-481C-BE82-8541B1C8E995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" activeCellId="1" sqref="D7 E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,7 +648,7 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="6">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -657,7 +657,7 @@
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="6">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -672,7 +672,7 @@
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C12" s="6">
         <f>(C3+C4+C5+C6+C7+C8+C9+C10+C11)/900*100</f>
-        <v>79.333333333333329</v>
+        <v>82.111111111111114</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
@@ -755,27 +755,27 @@
       <c r="A23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="3"/>
+      <c r="B23" s="2"/>
       <c r="C23" s="6">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="3"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="6">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="3"/>
+      <c r="B25" s="2"/>
       <c r="C25" s="6">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -790,7 +790,7 @@
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C27" s="6">
         <f>(C21+C22+C23+C24+C25+C26)/600*100</f>
-        <v>67.5</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
@@ -851,9 +851,9 @@
       <c r="A35" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B35" s="3"/>
+      <c r="B35" s="2"/>
       <c r="C35" s="6">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -871,13 +871,13 @@
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="6">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C38">
         <f>(C34+C35+C36+C37)/400*100</f>
-        <v>51.249999999999993</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.4">

</xml_diff>